<commit_message>
Corrected value of C61 in BOM
</commit_message>
<xml_diff>
--- a/DSpeed_v1.3/DStage_DSpeed_v1.3_BOM.xlsx
+++ b/DSpeed_v1.3/DStage_DSpeed_v1.3_BOM.xlsx
@@ -455,7 +455,7 @@
     <t>10n</t>
   </si>
   <si>
-    <t>C20, C21, C28</t>
+    <t>C20, C21, C28, C61</t>
   </si>
   <si>
     <t>C1710</t>
@@ -497,7 +497,7 @@
     <t>100n</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C3, C4, C5, C6, C24, C25, C26, C29, C30, C31, C32, C51, C60, C61, C75
+    <t xml:space="preserve">C1, C2, C3, C4, C5, C6, C24, C25, C26, C29, C30, C31, C32, C51, C60, C75
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Updated BOM with some fresh JLC codes, correct C61
</commit_message>
<xml_diff>
--- a/DSpeed_v1.3/DStage_DSpeed_v1.3_BOM.xlsx
+++ b/DSpeed_v1.3/DStage_DSpeed_v1.3_BOM.xlsx
@@ -467,7 +467,7 @@
     <t>10n</t>
   </si>
   <si>
-    <t>C20, C21, C28</t>
+    <t>C20, C21, C28, C61</t>
   </si>
   <si>
     <t>C1710</t>
@@ -509,7 +509,7 @@
     <t>100n</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C3, C4, C5, C6, C24, C25, C26, C29, C30, C31, C32, C51, C60, C61, C75
+    <t xml:space="preserve">C1, C2, C3, C4, C5, C6, C24, C25, C26, C29, C30, C31, C32, C51, C60, C75
 </t>
   </si>
   <si>
@@ -1707,7 +1707,7 @@
       <c r="A45" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="24" t="s">
         <v>151</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1773,7 +1773,7 @@
       <c r="A49" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="24" t="s">
         <v>165</v>
       </c>
       <c r="C49" s="12" t="s">

</xml_diff>